<commit_message>
Skip autoencoder and regularization experiments #8
</commit_message>
<xml_diff>
--- a/src/2.Experiments/results/Results.xlsx
+++ b/src/2.Experiments/results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Personal\Master Ciencia de Datos - UOC\TFM\Brain-MRI-Denoiser-Autoencoder\src\2.Experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BA3E2E-DBBB-407F-AE64-36108786DAE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89731242-653D-484B-A5CA-A16111C8E4AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32235" yWindow="4470" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Very Small ResCAE</t>
   </si>
   <si>
-    <t>BN in identity</t>
-  </si>
-  <si>
     <t>Normalization</t>
   </si>
   <si>
@@ -121,20 +118,50 @@
     <t>Myronenko encoder CAE</t>
   </si>
   <si>
-    <t>Only encoder - FPR</t>
-  </si>
-  <si>
     <t>INPUT SHAPE</t>
   </si>
   <si>
     <t>128x128x1</t>
+  </si>
+  <si>
+    <t>Cae+SkipConnections</t>
+  </si>
+  <si>
+    <t>16x16x129</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Sigmoid vs STD_norm</t>
+  </si>
+  <si>
+    <t>Regularizacion</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2 skip-connections</t>
+  </si>
+  <si>
+    <t>Full-pre ls128</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>BAD</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +225,27 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +329,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -293,10 +341,13 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
@@ -585,200 +636,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O8"/>
+  <dimension ref="B1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="13"/>
-    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="11" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H2" s="11"/>
-      <c r="I2" s="8" t="s">
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I2" s="12"/>
+      <c r="J2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="2:17" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.49</v>
+      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="16">
+        <v>1.111093E-4</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="16">
+        <v>3.9246999999999999E-5</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="14">
-        <v>3.9246999999999999E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="16">
+        <v>1.0972E-4</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="16">
+        <v>1.839338E-4</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1.4740063E-3</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="16">
+        <v>1.10335E-5</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -799,10 +1073,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script for TEST Metrics and Model Evaluation Automation #5
</commit_message>
<xml_diff>
--- a/src/2.Experiments/results/Results.xlsx
+++ b/src/2.Experiments/results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Personal\Master Ciencia de Datos - UOC\TFM\Brain-MRI-Denoiser-Autoencoder\src\2.Experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89731242-653D-484B-A5CA-A16111C8E4AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65279937-8F28-43B7-A591-4DD4D2895A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="44">
   <si>
     <t>Model</t>
   </si>
@@ -155,13 +155,16 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +249,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -322,6 +333,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -329,7 +358,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -339,15 +368,27 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
@@ -639,7 +680,7 @@
   <dimension ref="B1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +692,7 @@
     <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="10" customWidth="1"/>
     <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -664,7 +705,7 @@
       <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>28</v>
       </c>
       <c r="J1" s="5"/>
@@ -679,7 +720,7 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="I2" s="12"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="8" t="s">
         <v>22</v>
       </c>
@@ -715,31 +756,31 @@
       <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -753,7 +794,7 @@
       <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
@@ -762,28 +803,34 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="14">
         <v>0.49</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q4" s="14" t="s">
+      <c r="J4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -797,37 +844,39 @@
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="14">
         <v>1.111093E-4</v>
       </c>
-      <c r="J5" s="17"/>
+      <c r="J5" s="17">
+        <v>1.0945E-4</v>
+      </c>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" s="14" t="s">
+      <c r="N5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -841,7 +890,7 @@
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
@@ -850,28 +899,30 @@
       <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="14">
         <v>3.9246999999999999E-5</v>
       </c>
-      <c r="J6" s="17"/>
+      <c r="J6" s="17">
+        <v>3.8183699999999998E-5</v>
+      </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q6" s="14" t="s">
+      <c r="N6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -885,7 +936,7 @@
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
@@ -894,28 +945,30 @@
       <c r="G7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="14">
         <v>1.0972E-4</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="17">
+        <v>1.078119E-4</v>
+      </c>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" s="14" t="s">
+      <c r="N7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -929,7 +982,7 @@
       <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
@@ -938,28 +991,30 @@
       <c r="G8" t="s">
         <v>5</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="14">
         <v>1.839338E-4</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="17">
+        <v>1.810452E-4</v>
+      </c>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q8" s="14" t="s">
+      <c r="N8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -973,7 +1028,7 @@
       <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
@@ -982,28 +1037,30 @@
       <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="14">
         <v>1.4740063E-3</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="17">
+        <v>1.4799542E-3</v>
+      </c>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q9" s="14" t="s">
+      <c r="N9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1017,37 +1074,39 @@
       <c r="D10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="14">
         <v>1.10335E-5</v>
       </c>
-      <c r="J10" s="17"/>
+      <c r="J10" s="17">
+        <v>1.0669999999999999E-5</v>
+      </c>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q10" s="14" t="s">
+      <c r="N10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="16" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>